<commit_message>
Reassess aesdd, baum1, baum2
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/michen_ad_unc_edu/Documents/Desktop/multilingual_speech_valence_classification/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{9C4DCC86-0EEF-42A1-B41D-E15BA90F189F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CFEEE54D-A7FA-4925-A642-8CD9BA7DD242}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDAD69C-D5E6-4E87-8152-E2CCC7F50D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
   <si>
     <t>Lang.</t>
   </si>
@@ -82,9 +82,6 @@
     <t>acted + spon.</t>
   </si>
   <si>
-    <t>1 "improvised" sample per speaker</t>
-  </si>
-  <si>
     <t># neu.</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
     <t>fea</t>
   </si>
   <si>
-    <t>movie or TV; only 'useful' included; labeled by majority vote; 4 records excluded for interrater ambiguity (3 en 1 tr)</t>
-  </si>
-  <si>
     <t>from online talk shows; used unsegmented (utterance level); labels no good</t>
   </si>
   <si>
@@ -313,7 +307,19 @@
     <t>intrest</t>
   </si>
   <si>
-    <t>contempt mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!</t>
+    <t>1 "improvised" sample per speaker; actually 6 speakers</t>
+  </si>
+  <si>
+    <t>contempt, surprise, and boredom mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!; interest mapped to positive</t>
+  </si>
+  <si>
+    <t>movie or TV; excluded not useful audio; labeled by majority vote; 2 excluded for label mismatch or interrater ambiguity</t>
+  </si>
+  <si>
+    <t>movie or TV; excluded not useful audio; labeled by majority vote; 8 excluded for label mismatch or interrater ambiguity</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -329,12 +335,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -349,8 +361,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,9 +695,9 @@
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -696,7 +709,7 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -708,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -732,10 +745,10 @@
         <v>605</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -753,10 +766,10 @@
         <v/>
       </c>
       <c r="H3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -764,82 +777,82 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="D4">
-        <v>480</v>
+        <v>620</v>
       </c>
       <c r="E4">
         <v>185</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>864</v>
+        <v>1032</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D5">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D6">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -856,19 +869,22 @@
         <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
         <v>792</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -883,19 +899,19 @@
         <v>1063</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
         <v>6296</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -910,19 +926,19 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -937,19 +953,19 @@
         <v>221</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>1192</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -965,19 +981,19 @@
         <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
       <c r="H11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -992,19 +1008,19 @@
         <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>1102</v>
       </c>
       <c r="H12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1021,39 +1037,39 @@
         <v>142</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
       <c r="H13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1077,57 +1093,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1153,200 +1169,200 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1373,35 +1389,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1428,114 +1444,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data tsv for cafe and minor changes
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDAD69C-D5E6-4E87-8152-E2CCC7F50D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CA7E4A-C5CF-44B2-AF8B-FB940289DB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
   <si>
     <t>Lang.</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t>movie or TV; excluded not useful audio; labeled by majority vote; 8 excluded for label mismatch or interrater ambiguity</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -335,18 +332,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -363,7 +354,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +672,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,8 +852,7 @@
         <v>144</v>
       </c>
       <c r="D7">
-        <f>936-72-144-144</f>
-        <v>576</v>
+        <v>720</v>
       </c>
       <c r="E7">
         <f>6*12</f>
@@ -873,14 +863,12 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>792</v>
+        <v>936</v>
       </c>
       <c r="H7" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Update CREMA-D data org files and add the same for ekorpus and dzafic
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDAD69C-D5E6-4E87-8152-E2CCC7F50D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40746A22-7BCD-411E-93DF-9885582B7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
   <si>
     <t>Lang.</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Emotional_EMA</t>
   </si>
   <si>
-    <t>kept samples where intended valence matched multimodal reviewer consensus; where multimodal reviews classified ambiguous valence, labels recalculated; foreach remaining, where intended valence matches valence of highest emo score, keep those with scores &gt; 50</t>
-  </si>
-  <si>
     <t>perceived valence recoded from rater avg to ternary categorical majority vote; where no majority, avg used for recode; retained samples where new label matched intended valence; see formulae for counts by label method</t>
   </si>
   <si>
@@ -319,7 +316,7 @@
     <t>movie or TV; excluded not useful audio; labeled by majority vote; 8 excluded for label mismatch or interrater ambiguity</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>recoded intended emotions to valence; recoded fuzzy votes to valence; retained if rated valence in any of the three modalities matched intended valence</t>
   </si>
 </sst>
 </file>
@@ -335,18 +332,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -363,7 +354,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +672,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,7 +736,7 @@
         <v>605</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -766,7 +757,7 @@
         <v/>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -793,7 +784,7 @@
         <v>1032</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -820,7 +811,7 @@
         <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -847,7 +838,7 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -861,8 +852,7 @@
         <v>144</v>
       </c>
       <c r="D7">
-        <f>936-72-144-144</f>
-        <v>576</v>
+        <v>720</v>
       </c>
       <c r="E7">
         <f>6*12</f>
@@ -873,14 +863,12 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>792</v>
+        <v>936</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -890,23 +878,23 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>1218</v>
+        <v>1245</v>
       </c>
       <c r="D8">
-        <v>4015</v>
+        <v>4541</v>
       </c>
       <c r="E8">
-        <v>1063</v>
+        <v>1087</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>6296</v>
+        <v>6873</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -944,20 +932,20 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>296</v>
+        <v>232</v>
       </c>
       <c r="D10">
-        <v>675</v>
+        <v>493</v>
       </c>
       <c r="E10">
-        <v>221</v>
+        <v>142</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>1192</v>
+        <v>867</v>
       </c>
       <c r="H10" t="s">
         <v>53</v>
@@ -1044,12 +1032,12 @@
         <v>535</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1058,12 +1046,12 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1099,7 +1087,7 @@
         <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,7 +1098,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1121,7 +1109,7 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1132,7 +1120,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1143,7 +1131,7 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1163,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1186,7 +1174,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1197,7 +1185,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1208,7 +1196,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1219,7 +1207,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1230,7 +1218,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1241,7 +1229,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1252,7 +1240,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1263,7 +1251,7 @@
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1274,7 +1262,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1285,7 +1273,7 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1296,7 +1284,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1345,7 +1333,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
@@ -1356,7 +1344,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
         <v>61</v>
@@ -1395,7 +1383,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1406,7 +1394,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1417,7 +1405,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1536,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Add data org files for EmoDB and minor edits
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40746A22-7BCD-411E-93DF-9885582B7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249007B7-8C9D-4FE6-9EBE-F015733CB74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -247,9 +247,6 @@
     <t>sleepiness</t>
   </si>
   <si>
-    <t>included non-basic emotions, but all samples explicitly labeled for valence</t>
-  </si>
-  <si>
     <t>EmoReact_V_1.0</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>recoded intended emotions to valence; recoded fuzzy votes to valence; retained if rated valence in any of the three modalities matched intended valence</t>
+  </si>
+  <si>
+    <t>boredom is negative; data from kaggle link, not the one provided in the paper</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +736,7 @@
         <v>605</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -757,7 +757,7 @@
         <v/>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -784,7 +784,7 @@
         <v>1032</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -811,7 +811,7 @@
         <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -838,7 +838,7 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -866,7 +866,7 @@
         <v>936</v>
       </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -894,7 +894,7 @@
         <v>6873</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -976,12 +976,12 @@
         <v>535</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1003,12 +1003,12 @@
         <v>1102</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1032,12 +1032,12 @@
         <v>535</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1046,12 +1046,12 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1087,7 +1087,7 @@
         <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1098,7 +1098,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1109,7 +1109,7 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1120,7 +1120,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1131,7 +1131,7 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1163,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1174,7 +1174,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1185,7 +1185,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,7 +1196,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,7 +1207,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1218,7 +1218,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1229,7 +1229,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1240,7 +1240,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1251,7 +1251,7 @@
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1262,7 +1262,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1273,7 +1273,7 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1333,7 +1333,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
         <v>61</v>
@@ -1383,7 +1383,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1394,7 +1394,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Add data org files for Emotional_EMA and remove old old ones
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DCC482-3EE3-43C4-8BCD-988EFECC8518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9106915-6AA6-4824-B8C7-2A6412327CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
   <si>
     <t>Lang.</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Emotional_EMA</t>
   </si>
   <si>
-    <t>perceived valence recoded from rater avg to ternary categorical majority vote; where no majority, avg used for recode; retained samples where new label matched intended valence; see formulae for counts by label method</t>
-  </si>
-  <si>
     <t>EmoV-DB_sorted [en]</t>
   </si>
   <si>
@@ -317,6 +314,42 @@
   </si>
   <si>
     <t>N. A. children's English; see Notes.docx</t>
+  </si>
+  <si>
+    <t>perceived valence recoded to majority and average votes; if either matched intended valence, sample kept; discarded 58</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>bor</t>
+  </si>
+  <si>
+    <t>sur</t>
+  </si>
+  <si>
+    <t>uncertain</t>
+  </si>
+  <si>
+    <t>unc</t>
+  </si>
+  <si>
+    <t>frustration</t>
+  </si>
+  <si>
+    <t>fru</t>
+  </si>
+  <si>
+    <t>excitement</t>
+  </si>
+  <si>
+    <t>exc</t>
+  </si>
+  <si>
+    <t>curiosity</t>
+  </si>
+  <si>
+    <t>cur</t>
   </si>
 </sst>
 </file>
@@ -671,9 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -736,7 +767,7 @@
         <v>605</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -757,7 +788,7 @@
         <v/>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -784,7 +815,7 @@
         <v>1032</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -811,7 +842,7 @@
         <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -838,7 +869,7 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -866,7 +897,7 @@
         <v>936</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -894,7 +925,7 @@
         <v>6873</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -976,7 +1007,7 @@
         <v>535</v>
       </c>
       <c r="H11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1003,7 +1034,7 @@
         <v>912</v>
       </c>
       <c r="H12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1014,12 +1045,10 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <f>72+41</f>
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="D13">
-        <f>214+66</f>
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="E13">
         <v>142</v>
@@ -1029,15 +1058,15 @@
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>535</v>
+        <v>622</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1046,12 +1075,12 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1067,11 +1096,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1087,7 +1114,7 @@
         <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1098,7 +1125,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1109,7 +1136,7 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1120,7 +1147,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1131,7 +1158,51 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1144,11 +1215,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1163,7 +1232,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1174,7 +1243,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1185,7 +1254,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,7 +1265,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,7 +1276,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1218,7 +1287,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1229,7 +1298,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1240,7 +1309,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1251,7 +1320,7 @@
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1262,7 +1331,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1273,7 +1342,7 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1284,7 +1353,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1333,7 +1402,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
@@ -1344,13 +1413,101 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
         <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1365,9 +1522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1383,7 +1538,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1394,7 +1549,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1405,7 +1560,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1418,11 +1573,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA4603-F405-47FD-B096-17B0BE7B1580}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1440,7 +1593,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>61</v>
@@ -1448,7 +1601,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
@@ -1456,7 +1609,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
@@ -1464,7 +1617,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -1472,79 +1625,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B13">
-    <sortCondition ref="A1:A13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B7">
+    <sortCondition ref="A1:A7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update README.md and delete DATA.md
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9106915-6AA6-4824-B8C7-2A6412327CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8F817F-A5A1-4B83-A397-CE87ED2C443C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>Lang.</t>
   </si>
@@ -256,12 +256,6 @@
     <t>EmoV-DB_sorted [en]</t>
   </si>
   <si>
-    <t>EmoV-DB_sorted [fr]</t>
-  </si>
-  <si>
-    <t>elicitation prompts based on CMU Arctic (en) and SIWIS (fr)</t>
-  </si>
-  <si>
     <t>Québec French</t>
   </si>
   <si>
@@ -350,6 +344,9 @@
   </si>
   <si>
     <t>cur</t>
+  </si>
+  <si>
+    <t>elicitation prompts based on CMU Arctic (en) and SIWIS (fr); french samples are missing :(</t>
   </si>
 </sst>
 </file>
@@ -702,9 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -767,7 +766,7 @@
         <v>605</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -788,7 +787,7 @@
         <v/>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -815,7 +814,7 @@
         <v>1032</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -842,7 +841,7 @@
         <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -869,7 +868,7 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -897,7 +896,7 @@
         <v>936</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -925,7 +924,7 @@
         <v>6873</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1007,7 +1006,7 @@
         <v>535</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1034,7 +1033,7 @@
         <v>912</v>
       </c>
       <c r="H12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1061,7 +1060,7 @@
         <v>622</v>
       </c>
       <c r="H13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1075,18 +1074,7 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1102,7 @@
         <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1125,7 +1113,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1136,7 +1124,7 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1147,7 +1135,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1158,7 +1146,7 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1169,40 +1157,40 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1220,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1243,7 +1231,7 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1254,7 +1242,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1265,7 +1253,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1276,7 +1264,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1287,7 +1275,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1298,7 +1286,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1309,7 +1297,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1320,7 +1308,7 @@
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1331,7 +1319,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1342,7 +1330,7 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1353,7 +1341,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1402,7 +1390,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
@@ -1413,7 +1401,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
         <v>61</v>
@@ -1430,7 +1418,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1441,7 +1429,7 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1452,7 +1440,7 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1463,7 +1451,7 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1474,7 +1462,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1485,29 +1473,29 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
         <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1538,7 +1526,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1549,7 +1537,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1560,7 +1548,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix .gitignores and BAUM names
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8F817F-A5A1-4B83-A397-CE87ED2C443C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A1319-D737-4477-B9B8-6F6CC2797D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
   <si>
     <t>Lang.</t>
   </si>
@@ -292,9 +292,6 @@
     <t>1 "improvised" sample per speaker; actually 6 speakers</t>
   </si>
   <si>
-    <t>contempt, surprise, and boredom mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!; interest mapped to positive</t>
-  </si>
-  <si>
     <t>movie or TV; excluded not useful audio; labeled by majority vote; 2 excluded for label mismatch or interrater ambiguity</t>
   </si>
   <si>
@@ -347,6 +344,12 @@
   </si>
   <si>
     <t>elicitation prompts based on CMU Arctic (en) and SIWIS (fr); french samples are missing :(</t>
+  </si>
+  <si>
+    <t>bot</t>
+  </si>
+  <si>
+    <t>contempt, surprise, unsure, and boredom mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!; interest mapped to positive</t>
   </si>
 </sst>
 </file>
@@ -702,7 +705,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +804,7 @@
         <v>227</v>
       </c>
       <c r="D4">
-        <v>620</v>
+        <v>880</v>
       </c>
       <c r="E4">
         <v>185</v>
@@ -811,10 +814,10 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1032</v>
+        <v>1292</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -841,7 +844,7 @@
         <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -868,7 +871,7 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -924,7 +927,7 @@
         <v>6873</v>
       </c>
       <c r="H8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1006,7 +1009,7 @@
         <v>535</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1033,7 +1036,7 @@
         <v>912</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1060,7 +1063,7 @@
         <v>622</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1074,7 +1077,7 @@
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1157,7 +1160,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1168,29 +1171,29 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>98</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
         <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1203,9 +1206,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1418,7 +1423,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1429,7 +1434,7 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1440,7 +1445,7 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1451,7 +1456,7 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1462,7 +1467,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1473,29 +1478,40 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
         <v>94</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
         <v>96</v>
       </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>97</v>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1561,7 +1577,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA4603-F405-47FD-B096-17B0BE7B1580}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1581,7 +1597,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>61</v>
@@ -1589,7 +1605,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
@@ -1597,7 +1613,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
@@ -1605,23 +1621,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B7">
-    <sortCondition ref="A1:A7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B6">
+    <sortCondition ref="A1:A6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix collected records for BAUM1
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A1319-D737-4477-B9B8-6F6CC2797D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBED35-B6AB-48A6-AA66-F7F64E642914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -349,7 +349,7 @@
     <t>bot</t>
   </si>
   <si>
-    <t>contempt, surprise, unsure, and boredom mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!; interest mapped to positive</t>
+    <t>contempt, surprise, unsure, and boredom mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!; interest mapped to positive; 61 records missing labels dropped</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,10 +801,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D4">
-        <v>880</v>
+        <v>891</v>
       </c>
       <c r="E4">
         <v>185</v>
@@ -814,7 +814,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1292</v>
+        <v>1304</v>
       </c>
       <c r="H4" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Add data organization files for emotional voices db
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBED35-B6AB-48A6-AA66-F7F64E642914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A5E01F-D58D-4281-8FFC-EE4459425073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="104">
   <si>
     <t>Lang.</t>
   </si>
@@ -310,9 +310,6 @@
     <t>perceived valence recoded to majority and average votes; if either matched intended valence, sample kept; discarded 58</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>bor</t>
   </si>
   <si>
@@ -343,13 +340,16 @@
     <t>cur</t>
   </si>
   <si>
-    <t>elicitation prompts based on CMU Arctic (en) and SIWIS (fr); french samples are missing :(</t>
-  </si>
-  <si>
     <t>bot</t>
   </si>
   <si>
     <t>contempt, surprise, unsure, and boredom mapped to negative; labels determined by interrater consensus; some of the mp4s might not have audio!; interest mapped to positive; 61 records missing labels dropped</t>
+  </si>
+  <si>
+    <t>amu</t>
+  </si>
+  <si>
+    <t>elicitation prompts based on CMU Arctic (en) and SIWIS (fr); french samples are missing :(; only 3 emos available for josh</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +765,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G13" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
+        <f t="shared" ref="G2:G14" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
         <v>605</v>
       </c>
       <c r="H2" t="s">
@@ -817,7 +817,7 @@
         <v>1304</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1073,11 +1073,24 @@
       <c r="B14" t="s">
         <v>4</v>
       </c>
+      <c r="C14">
+        <v>1317</v>
+      </c>
+      <c r="D14">
+        <v>2287</v>
+      </c>
+      <c r="E14">
+        <v>1568</v>
+      </c>
       <c r="F14" t="s">
         <v>35</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>5172</v>
+      </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1087,9 +1100,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1160,7 +1175,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1171,29 +1186,40 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
         <v>99</v>
       </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>100</v>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1209,7 +1235,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,7 +1449,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,7 +1460,7 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1445,7 +1471,7 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1456,7 +1482,7 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1467,7 +1493,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1478,29 +1504,29 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
         <v>93</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
         <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1511,7 +1537,7 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data organization files for enterface db
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A5E01F-D58D-4281-8FFC-EE4459425073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07DBC45-A3C6-41BD-98DD-0A69B0FC486C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
   <si>
     <t>Lang.</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>elicitation prompts based on CMU Arctic (en) and SIWIS (fr); french samples are missing :(; only 3 emos available for josh</t>
+  </si>
+  <si>
+    <t>enterface_db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elicited in lab; </t>
   </si>
 </sst>
 </file>
@@ -702,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +771,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G14" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
+        <f t="shared" ref="G2:G16" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
         <v>605</v>
       </c>
       <c r="H2" t="s">
@@ -1091,6 +1097,39 @@
       </c>
       <c r="H14" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>213</v>
+      </c>
+      <c r="D15">
+        <v>1080</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1293</v>
+      </c>
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Specify iso 3166-1 locale codes
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07DBC45-A3C6-41BD-98DD-0A69B0FC486C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B6E50-860F-404C-9349-A774CB2F0462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
   <si>
     <t>Lang.</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t xml:space="preserve">elicited in lab; </t>
+  </si>
+  <si>
+    <t>esd</t>
+  </si>
+  <si>
+    <t>English and Mandarin</t>
   </si>
 </sst>
 </file>
@@ -711,7 +717,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,9 +1133,18 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+      <c r="H16" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data organization files for ESD
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B6E50-860F-404C-9349-A774CB2F0462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54EC5E-34DD-42D5-A7D8-91C988F589A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
   <si>
     <t>Lang.</t>
   </si>
@@ -358,10 +358,16 @@
     <t xml:space="preserve">elicited in lab; </t>
   </si>
   <si>
-    <t>esd</t>
-  </si>
-  <si>
     <t>English and Mandarin</t>
+  </si>
+  <si>
+    <t>esd [en]</t>
+  </si>
+  <si>
+    <t>esd [zh]</t>
+  </si>
+  <si>
+    <t>Mandarin Chinese</t>
   </si>
 </sst>
 </file>
@@ -714,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +733,7 @@
     <col min="3" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -777,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G16" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
+        <f t="shared" ref="G2:G17" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
         <v>605</v>
       </c>
       <c r="H2" t="s">
@@ -1134,17 +1140,56 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="G16" t="str">
+      <c r="C16">
+        <v>3500</v>
+      </c>
+      <c r="D16">
+        <v>10500</v>
+      </c>
+      <c r="E16">
+        <v>3500</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="0"/>
-        <v/>
+        <v>17500</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>3500</v>
+      </c>
+      <c r="D17">
+        <v>10500</v>
+      </c>
+      <c r="E17">
+        <v>3500</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="H17" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data organization files for EYASE
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54EC5E-34DD-42D5-A7D8-91C988F589A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D63569-EF5B-4512-A19D-737466B527CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
   <si>
     <t>Lang.</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>Mandarin Chinese</t>
+  </si>
+  <si>
+    <t>EYASE</t>
+  </si>
+  <si>
+    <t>Egyptian Arabic from a TV drama</t>
   </si>
 </sst>
 </file>
@@ -720,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,7 +789,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G17" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
+        <f t="shared" ref="G2:G19" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
         <v>605</v>
       </c>
       <c r="H2" t="s">
@@ -1190,6 +1196,39 @@
       </c>
       <c r="H17" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>132</v>
+      </c>
+      <c r="D18">
+        <v>297</v>
+      </c>
+      <c r="E18">
+        <v>150</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>579</v>
+      </c>
+      <c r="H18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1702,9 +1741,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA4603-F405-47FD-B096-17B0BE7B1580}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1714,7 +1755,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
@@ -1722,7 +1763,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>61</v>
@@ -1730,7 +1771,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
@@ -1738,23 +1779,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B6">
-    <sortCondition ref="A1:A6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B5">
+    <sortCondition ref="A1:A5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add data organization files for jl-corpus
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D63569-EF5B-4512-A19D-737466B527CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FFEB51-C793-41CF-ACCC-4B79011463F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="128">
   <si>
     <t>Lang.</t>
   </si>
@@ -374,6 +374,54 @@
   </si>
   <si>
     <t>Egyptian Arabic from a TV drama</t>
+  </si>
+  <si>
+    <t>jl-corpus</t>
+  </si>
+  <si>
+    <t>pensive</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>enthusiastic</t>
+  </si>
+  <si>
+    <t>ent</t>
+  </si>
+  <si>
+    <t>apologetic</t>
+  </si>
+  <si>
+    <t>apo</t>
+  </si>
+  <si>
+    <t>anxious</t>
+  </si>
+  <si>
+    <t>anx</t>
+  </si>
+  <si>
+    <t>worried</t>
+  </si>
+  <si>
+    <t>wor</t>
+  </si>
+  <si>
+    <t>excited</t>
+  </si>
+  <si>
+    <t>encouraging</t>
+  </si>
+  <si>
+    <t>concerned</t>
+  </si>
+  <si>
+    <t>assertive</t>
+  </si>
+  <si>
+    <t>New Zealand English; valence labels were provided for the non-primary emotions; semi-natural elicitation (almost spont.); apologetic, anxious, worried negative; excited and happy positive</t>
   </si>
 </sst>
 </file>
@@ -729,7 +777,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,9 +1274,30 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G19" t="str">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>480</v>
+      </c>
+      <c r="D19">
+        <v>960</v>
+      </c>
+      <c r="E19">
+        <v>240</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1680</v>
+      </c>
+      <c r="H19" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1238,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1360,6 +1429,39 @@
         <v>102</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B5">
     <sortCondition ref="A2:A5"/>
@@ -1370,11 +1472,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1676,6 +1776,39 @@
       </c>
       <c r="C27" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1741,11 +1874,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA4603-F405-47FD-B096-17B0BE7B1580}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1785,6 +1916,30 @@
         <v>61</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B5">
     <sortCondition ref="A1:A5"/>

</xml_diff>

<commit_message>
Add data organization files for LEGOv2
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FFEB51-C793-41CF-ACCC-4B79011463F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEF4C21-B722-4D70-9D6F-8D6B4A3BC1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="130">
   <si>
     <t>Lang.</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>New Zealand English; valence labels were provided for the non-primary emotions; semi-natural elicitation (almost spont.); apologetic, anxious, worried negative; excited and happy positive</t>
+  </si>
+  <si>
+    <t>LEGOv2</t>
+  </si>
+  <si>
+    <t>from an automated bus info service</t>
   </si>
 </sst>
 </file>
@@ -774,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,7 +843,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G19" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
+        <f t="shared" ref="G2:G28" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
         <v>605</v>
       </c>
       <c r="H2" t="s">
@@ -1298,6 +1304,81 @@
       </c>
       <c r="H19" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>797</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>797</v>
+      </c>
+      <c r="H20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start tracking speaker IDs
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEF4C21-B722-4D70-9D6F-8D6B4A3BC1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CFDDD6-6044-45EA-B14D-2AEEAEAB184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="133">
   <si>
     <t>Lang.</t>
   </si>
@@ -427,7 +427,16 @@
     <t>LEGOv2</t>
   </si>
   <si>
-    <t>from an automated bus info service</t>
+    <t>MELD</t>
+  </si>
+  <si>
+    <t>unique speakers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [tr+en]</t>
+  </si>
+  <si>
+    <t>from an automated bus info service; some unknown gender labels</t>
   </si>
 </sst>
 </file>
@@ -780,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,10 +803,11 @@
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -820,10 +830,13 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -846,11 +859,14 @@
         <f t="shared" ref="G2:G28" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
         <v>605</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -867,11 +883,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -894,11 +910,14 @@
         <f t="shared" si="0"/>
         <v>1304</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -921,11 +940,14 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>147</v>
+      </c>
+      <c r="I5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -949,10 +971,13 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -976,12 +1001,15 @@
         <f t="shared" si="0"/>
         <v>936</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1004,11 +1032,14 @@
         <f t="shared" si="0"/>
         <v>6873</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>91</v>
+      </c>
+      <c r="I8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1031,11 +1062,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1058,11 +1092,14 @@
         <f t="shared" si="0"/>
         <v>867</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1086,11 +1123,14 @@
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1113,11 +1153,14 @@
         <f t="shared" si="0"/>
         <v>912</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <v>63</v>
+      </c>
+      <c r="I12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1140,11 +1183,14 @@
         <f t="shared" si="0"/>
         <v>622</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -1167,11 +1213,14 @@
         <f t="shared" si="0"/>
         <v>5172</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1194,11 +1243,14 @@
         <f t="shared" si="0"/>
         <v>1293</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15">
+        <v>44</v>
+      </c>
+      <c r="I15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -1221,11 +1273,14 @@
         <f t="shared" si="0"/>
         <v>17500</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -1248,11 +1303,14 @@
         <f t="shared" si="0"/>
         <v>17500</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>110</v>
       </c>
@@ -1275,11 +1333,14 @@
         <f t="shared" si="0"/>
         <v>579</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -1302,11 +1363,14 @@
         <f t="shared" si="0"/>
         <v>1680</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>128</v>
       </c>
@@ -1329,53 +1393,59 @@
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20">
+        <v>134</v>
+      </c>
+      <c r="I20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Fix EmoReact ambiguities, remove some old notes, and update a gitignore's comments
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CFDDD6-6044-45EA-B14D-2AEEAEAB184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EED354-52BD-4229-A246-5D05B431E4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_retained" sheetId="1" r:id="rId1"/>
-    <sheet name="positive" sheetId="2" r:id="rId2"/>
-    <sheet name="negative" sheetId="3" r:id="rId3"/>
-    <sheet name="neutral" sheetId="5" r:id="rId4"/>
-    <sheet name="discard" sheetId="4" r:id="rId5"/>
+    <sheet name="multi-valenced" sheetId="6" r:id="rId2"/>
+    <sheet name="positive" sheetId="2" r:id="rId3"/>
+    <sheet name="negative" sheetId="3" r:id="rId4"/>
+    <sheet name="neutral" sheetId="5" r:id="rId5"/>
+    <sheet name="discard" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
   <si>
     <t>Lang.</t>
   </si>
@@ -304,9 +305,6 @@
     <t>boredom is negative; data from kaggle link, not the one provided in the paper</t>
   </si>
   <si>
-    <t>N. A. children's English; see Notes.docx</t>
-  </si>
-  <si>
     <t>perceived valence recoded to majority and average votes; if either matched intended valence, sample kept; discarded 58</t>
   </si>
   <si>
@@ -355,12 +353,6 @@
     <t>enterface_db</t>
   </si>
   <si>
-    <t xml:space="preserve">elicited in lab; </t>
-  </si>
-  <si>
-    <t>English and Mandarin</t>
-  </si>
-  <si>
     <t>esd [en]</t>
   </si>
   <si>
@@ -421,9 +413,6 @@
     <t>assertive</t>
   </si>
   <si>
-    <t>New Zealand English; valence labels were provided for the non-primary emotions; semi-natural elicitation (almost spont.); apologetic, anxious, worried negative; excited and happy positive</t>
-  </si>
-  <si>
     <t>LEGOv2</t>
   </si>
   <si>
@@ -436,7 +425,76 @@
     <t xml:space="preserve"> [tr+en]</t>
   </si>
   <si>
-    <t>from an automated bus info service; some unknown gender labels</t>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>orig. emotions</t>
+  </si>
+  <si>
+    <t>Anger, Boredom, Bothered, Concentrating, Contempt, Disgust, Fear, Happiness, Interest, Neutral, Sadness, Surprise, Thinking, Unsure</t>
+  </si>
+  <si>
+    <t>Angry, contempt, disgust, fear, happy, neutral, sadness, surprise</t>
+  </si>
+  <si>
+    <t>anger, disgust, joy, neutral, fear, surprise, sadness</t>
+  </si>
+  <si>
+    <t>Anger, Disgust, Fear, Happy, Neutral, Sad</t>
+  </si>
+  <si>
+    <t>angry, happy, neutral</t>
+  </si>
+  <si>
+    <t>joy, anger, sadness, neutral</t>
+  </si>
+  <si>
+    <t>neutral, anger, fear, joy, sadness, disgust, boredom</t>
+  </si>
+  <si>
+    <t>curiosity, excitement, happiness, uncertainty, surprise, disgust, fear, frustration; exploration, confusion, anxiety, attentiveness, anger, sadness, embarrassment</t>
+  </si>
+  <si>
+    <t>happy, angry, sad, neutral others</t>
+  </si>
+  <si>
+    <t>amused, angry, disgusted, neutral, sleepy</t>
+  </si>
+  <si>
+    <t>anger, disgust, fear, happiness, sadness, surprise</t>
+  </si>
+  <si>
+    <t>elicited in lab; surprise mapped to negative for this one</t>
+  </si>
+  <si>
+    <t>happy, sad, neutral, angry, surprise</t>
+  </si>
+  <si>
+    <t>English and Mandarin; surprise mapped negative for this one</t>
+  </si>
+  <si>
+    <t>angry, happy, neutral, sad</t>
+  </si>
+  <si>
+    <t>angry, anxious, neutral, sad, worried, apologetic, pensive, excited, enthusiastic,  happy</t>
+  </si>
+  <si>
+    <t>very angry, slightly angry, non-angry</t>
+  </si>
+  <si>
+    <t>only angry</t>
+  </si>
+  <si>
+    <t>New Zealand English; valence labels were provided for the non-primary emotions; semi-natural elicitation (almost spont.); apologetic, anxious, worried negative; excited and happy positive; not all present</t>
+  </si>
+  <si>
+    <t>anger, disgust, fear, happiness, sadness</t>
+  </si>
+  <si>
+    <t>N. A. children's English; see Notes.docx; contains mixed-valence curious including neutral valence</t>
   </si>
 </sst>
 </file>
@@ -792,7 +850,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +862,7 @@
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -830,9 +888,12 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
         <v>130</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -863,6 +924,9 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -883,7 +947,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -914,7 +978,10 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>101</v>
+        <v>131</v>
+      </c>
+      <c r="J4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -944,6 +1011,9 @@
         <v>147</v>
       </c>
       <c r="I5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -971,9 +1041,12 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1004,10 +1077,12 @@
       <c r="H7">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J7" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1035,7 +1110,10 @@
       <c r="H8">
         <v>91</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1065,7 +1143,10 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1095,7 +1176,10 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1126,7 +1210,10 @@
       <c r="H11">
         <v>10</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1138,10 +1225,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>579</v>
+        <v>523</v>
       </c>
       <c r="D12">
-        <v>295</v>
+        <v>376</v>
       </c>
       <c r="E12">
         <v>38</v>
@@ -1151,13 +1238,16 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>912</v>
+        <v>937</v>
       </c>
       <c r="H12">
         <v>63</v>
       </c>
-      <c r="I12" t="s">
-        <v>88</v>
+      <c r="I12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1186,8 +1276,11 @@
       <c r="H13">
         <v>3</v>
       </c>
-      <c r="I13" t="s">
-        <v>89</v>
+      <c r="I13" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1216,13 +1309,16 @@
       <c r="H14">
         <v>4</v>
       </c>
-      <c r="I14" t="s">
-        <v>103</v>
+      <c r="I14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1246,13 +1342,16 @@
       <c r="H15">
         <v>44</v>
       </c>
-      <c r="I15" t="s">
-        <v>105</v>
+      <c r="I15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -1276,13 +1375,16 @@
       <c r="H16">
         <v>10</v>
       </c>
-      <c r="I16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -1297,7 +1399,7 @@
         <v>3500</v>
       </c>
       <c r="F17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -1306,13 +1408,16 @@
       <c r="H17">
         <v>10</v>
       </c>
-      <c r="I17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -1336,13 +1441,16 @@
       <c r="H18">
         <v>6</v>
       </c>
-      <c r="I18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -1366,13 +1474,16 @@
       <c r="H19">
         <v>4</v>
       </c>
-      <c r="I19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1396,56 +1507,59 @@
       <c r="H20">
         <v>134</v>
       </c>
-      <c r="I20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1457,11 +1571,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4FBC7C-E990-492C-91F7-722D544A6419}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,7 +1716,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1544,73 +1727,62 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
         <v>113</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
         <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1621,9 +1793,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1838,7 +2010,7 @@
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1849,117 +2021,84 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
         <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
         <v>119</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +2109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2023,7 +2162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA4603-F405-47FD-B096-17B0BE7B1580}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2069,7 +2208,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -2077,7 +2216,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
         <v>61</v>
@@ -2085,7 +2224,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Add data organization files for MELD
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EED354-52BD-4229-A246-5D05B431E4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257C9C2F-6BC3-48DC-98DE-FE96DD427970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
   <si>
     <t>Lang.</t>
   </si>
@@ -495,14 +495,43 @@
   </si>
   <si>
     <t>N. A. children's English; see Notes.docx; contains mixed-valence curious including neutral valence</t>
+  </si>
+  <si>
+    <r>
+      <t>Friends</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> data</t>
+    </r>
+  </si>
+  <si>
+    <t>Joy, Sadness, Fear, Anger, Surprise, Disgust, Neutral</t>
+  </si>
+  <si>
+    <t>oreau2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -530,9 +559,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,7 +880,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,12 +1548,42 @@
       <c r="A21" t="s">
         <v>125</v>
       </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3086</v>
+      </c>
+      <c r="D21">
+        <v>4186</v>
+      </c>
+      <c r="E21">
+        <v>6430</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>13702</v>
+      </c>
+      <c r="H21">
+        <v>356</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
+      </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1567,6 +1627,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add data organization files for oreau2
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257C9C2F-6BC3-48DC-98DE-FE96DD427970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563C9AAF-2DBB-4BAF-A5EC-7F9C48FF6084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="161">
   <si>
     <t>Lang.</t>
   </si>
@@ -516,6 +516,24 @@
   </si>
   <si>
     <t>oreau2</t>
+  </si>
+  <si>
+    <t>ravdess</t>
+  </si>
+  <si>
+    <t>savee</t>
+  </si>
+  <si>
+    <t>ShEMO</t>
+  </si>
+  <si>
+    <t>tess</t>
+  </si>
+  <si>
+    <t>urdu</t>
+  </si>
+  <si>
+    <t>vivae</t>
   </si>
 </sst>
 </file>
@@ -880,7 +898,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1581,45 +1599,81 @@
       <c r="A22" t="s">
         <v>154</v>
       </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>62</v>
+      </c>
+      <c r="D22">
+        <v>302</v>
+      </c>
+      <c r="E22">
+        <v>70</v>
+      </c>
       <c r="F22" t="s">
         <v>37</v>
       </c>
-      <c r="G22" t="str">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>434</v>
+      </c>
+      <c r="H22">
+        <v>32</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G23" t="str">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G24" t="str">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G25" t="str">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>158</v>
+      </c>
+      <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G26" t="str">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+      <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Apply a small edit to readme and add data organization files for ravdess
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563C9AAF-2DBB-4BAF-A5EC-7F9C48FF6084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B975FFC5-4B7D-4029-94FF-9147262FBC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_retained" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="165">
   <si>
     <t>Lang.</t>
   </si>
@@ -534,6 +534,18 @@
   </si>
   <si>
     <t>vivae</t>
+  </si>
+  <si>
+    <t>neutral, calm, happy, sad, angry, fearful, surprise, and disgust</t>
+  </si>
+  <si>
+    <t>calm -&gt; 0 here, North American (Canadian) English; contains emotional song samples</t>
+  </si>
+  <si>
+    <t>calm</t>
+  </si>
+  <si>
+    <t>cal</t>
   </si>
 </sst>
 </file>
@@ -897,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1629,9 +1641,33 @@
       <c r="A23" t="s">
         <v>155</v>
       </c>
-      <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>376</v>
+      </c>
+      <c r="D23">
+        <v>1512</v>
+      </c>
+      <c r="E23">
+        <v>564</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>2452</v>
+      </c>
+      <c r="H23">
+        <v>24</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2226,9 +2262,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2267,6 +2305,17 @@
       </c>
       <c r="C3" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data organization files for savee and update gitignore files
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B975FFC5-4B7D-4029-94FF-9147262FBC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C7CD45-1E5E-473B-9827-70DD4F615322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_retained" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
   <si>
     <t>Lang.</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>cal</t>
+  </si>
+  <si>
+    <t>anger, disgust, fear, happiness, neutral, sadness, surprise</t>
+  </si>
+  <si>
+    <t>added more unique speakers from MetaData folder; 4 main male speakers otherwise</t>
   </si>
 </sst>
 </file>
@@ -909,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1674,9 +1680,34 @@
       <c r="A24" t="s">
         <v>156</v>
       </c>
-      <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>61</v>
+      </c>
+      <c r="D24">
+        <v>306</v>
+      </c>
+      <c r="E24">
+        <v>121</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>488</v>
+      </c>
+      <c r="H24">
+        <f>4+7</f>
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>165</v>
+      </c>
+      <c r="J24" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2264,7 +2295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add data organization files for ShEMO
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C7CD45-1E5E-473B-9827-70DD4F615322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B0FC2-B260-4D64-A46E-700B1E998B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_retained" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="170">
   <si>
     <t>Lang.</t>
   </si>
@@ -552,6 +552,15 @@
   </si>
   <si>
     <t>added more unique speakers from MetaData folder; 4 main male speakers otherwise</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>anger, happiness, neutrality, sadness, surprise, fear</t>
+  </si>
+  <si>
+    <t>Iranian Persian</t>
   </si>
 </sst>
 </file>
@@ -916,7 +925,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,9 +1723,33 @@
       <c r="A25" t="s">
         <v>157</v>
       </c>
-      <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>201</v>
+      </c>
+      <c r="D25">
+        <v>1771</v>
+      </c>
+      <c r="E25">
+        <v>1028</v>
+      </c>
+      <c r="F25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="H25">
+        <v>87</v>
+      </c>
+      <c r="I25" t="s">
+        <v>168</v>
+      </c>
+      <c r="J25" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add data organization files for tess
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B0FC2-B260-4D64-A46E-700B1E998B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255B344A-5B4D-4543-A491-14E867806AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_retained" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="173">
   <si>
     <t>Lang.</t>
   </si>
@@ -561,6 +561,15 @@
   </si>
   <si>
     <t>Iranian Persian</t>
+  </si>
+  <si>
+    <t>Toronto English</t>
+  </si>
+  <si>
+    <t>anger, disgust, fear, happiness, pleasant surprise, sadness, neutral</t>
+  </si>
+  <si>
+    <t>Discourse or standalone</t>
   </si>
 </sst>
 </file>
@@ -922,285 +931,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>130</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>119</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>486</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G28" si="0">IF(OR(ISBLANK(C2), ISBLANK(D2),ISBLANK(E2)), "", SUM(C2:E2))</f>
+      <c r="H2">
+        <f t="shared" ref="H2:H28" si="0">IF(OR(ISBLANK(D2), ISBLANK(E2),ISBLANK(F2)), "", SUM(D2:F2))</f>
         <v>605</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>150</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>228</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>891</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>185</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>1304</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>131</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>36</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>86</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>147</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>132</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>49</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
       </c>
       <c r="E6">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>127</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>132</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>144</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>720</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f>6*12</f>
         <v>72</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>936</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>12</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1245</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>4541</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1087</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>6873</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>91</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>4</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1208,573 +1216,600 @@
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
         <v>35</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>232</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>493</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>142</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>55</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>867</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>56</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>71</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f>535-(79+71)</f>
         <v>385</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>79</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>58</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>523</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>376</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>38</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>35</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>937</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>63</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>147</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>333</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>142</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>35</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>622</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>3</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>1317</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2287</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1568</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>35</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>5172</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>4</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>213</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>1080</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>35</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>1293</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>44</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>104</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>3500</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>10500</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>3500</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>35</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>17500</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>10</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>105</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>3500</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>10500</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>3500</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>106</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>17500</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>10</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>107</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>132</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>297</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>150</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>10</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>579</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>6</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>109</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>480</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>960</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>240</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>35</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>1680</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>4</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>124</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>797</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>35</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>134</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>125</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>3086</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>4186</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>6430</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>35</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>13702</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>356</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>154</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>62</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>302</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>70</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>37</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>434</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>32</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>155</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>376</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>1512</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>564</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>35</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>2452</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>24</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>156</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="C24">
-        <v>61</v>
-      </c>
       <c r="D24">
+        <v>61</v>
+      </c>
+      <c r="E24">
         <v>306</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>121</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>35</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="0"/>
         <v>488</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f>4+7</f>
         <v>11</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>165</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>157</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>201</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>1771</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>1028</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>167</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>87</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>168</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>158</v>
       </c>
-      <c r="G26" t="str">
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>800</v>
+      </c>
+      <c r="E26">
+        <v>1600</v>
+      </c>
+      <c r="F26">
+        <v>400</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>171</v>
+      </c>
+      <c r="K26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>159</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>160</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Start tracking whether recordings were sampled from a discourse or non-discourse context
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255B344A-5B4D-4543-A491-14E867806AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DE8932-4E1D-4600-A800-87238592BB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="176">
   <si>
     <t>Lang.</t>
   </si>
@@ -551,9 +551,6 @@
     <t>anger, disgust, fear, happiness, neutral, sadness, surprise</t>
   </si>
   <si>
-    <t>added more unique speakers from MetaData folder; 4 main male speakers otherwise</t>
-  </si>
-  <si>
     <t>Persian</t>
   </si>
   <si>
@@ -563,13 +560,25 @@
     <t>Iranian Persian</t>
   </si>
   <si>
-    <t>Toronto English</t>
-  </si>
-  <si>
     <t>anger, disgust, fear, happiness, pleasant surprise, sadness, neutral</t>
   </si>
   <si>
-    <t>Discourse or standalone</t>
+    <t>discourse</t>
+  </si>
+  <si>
+    <t>non-discourse</t>
+  </si>
+  <si>
+    <t>elicited from discourse</t>
+  </si>
+  <si>
+    <t>not to be confused with v1</t>
+  </si>
+  <si>
+    <t>added more unique speakers from MetaData folder; 4 main male speakers otherwise; the MetaData samples are arguably sampled from a discourse context</t>
+  </si>
+  <si>
+    <t>Toronto English; single words</t>
   </si>
 </sst>
 </file>
@@ -933,7 +942,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -987,6 +998,9 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1041,6 +1055,9 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -1074,6 +1091,9 @@
       <c r="A5" t="s">
         <v>33</v>
       </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1107,6 +1127,9 @@
       <c r="A6" t="s">
         <v>34</v>
       </c>
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -1140,6 +1163,9 @@
       <c r="A7" t="s">
         <v>36</v>
       </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -1174,6 +1200,9 @@
       <c r="A8" t="s">
         <v>48</v>
       </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -1207,6 +1236,9 @@
       <c r="A9" t="s">
         <v>50</v>
       </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -1240,6 +1272,9 @@
       <c r="A10" t="s">
         <v>52</v>
       </c>
+      <c r="B10" t="s">
+        <v>171</v>
+      </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -1273,6 +1308,9 @@
       <c r="A11" t="s">
         <v>56</v>
       </c>
+      <c r="B11" t="s">
+        <v>171</v>
+      </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -1307,6 +1345,9 @@
       <c r="A12" t="s">
         <v>69</v>
       </c>
+      <c r="B12" t="s">
+        <v>170</v>
+      </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
@@ -1340,6 +1381,9 @@
       <c r="A13" t="s">
         <v>70</v>
       </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
@@ -1373,6 +1417,9 @@
       <c r="A14" t="s">
         <v>71</v>
       </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
@@ -1406,6 +1453,9 @@
       <c r="A15" t="s">
         <v>103</v>
       </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -1439,6 +1489,9 @@
       <c r="A16" t="s">
         <v>104</v>
       </c>
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
@@ -1472,6 +1525,9 @@
       <c r="A17" t="s">
         <v>105</v>
       </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
@@ -1505,6 +1561,9 @@
       <c r="A18" t="s">
         <v>107</v>
       </c>
+      <c r="B18" t="s">
+        <v>170</v>
+      </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -1538,6 +1597,9 @@
       <c r="A19" t="s">
         <v>109</v>
       </c>
+      <c r="B19" t="s">
+        <v>171</v>
+      </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
@@ -1571,6 +1633,9 @@
       <c r="A20" t="s">
         <v>124</v>
       </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
@@ -1604,6 +1669,9 @@
       <c r="A21" t="s">
         <v>125</v>
       </c>
+      <c r="B21" t="s">
+        <v>170</v>
+      </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
@@ -1637,6 +1705,9 @@
       <c r="A22" t="s">
         <v>154</v>
       </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
@@ -1662,11 +1733,17 @@
       <c r="J22" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="K22" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>155</v>
       </c>
+      <c r="B23" t="s">
+        <v>171</v>
+      </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
@@ -1700,6 +1777,9 @@
       <c r="A24" t="s">
         <v>156</v>
       </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
@@ -1727,13 +1807,16 @@
         <v>165</v>
       </c>
       <c r="K24" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>157</v>
       </c>
+      <c r="B25" t="s">
+        <v>170</v>
+      </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
@@ -1747,7 +1830,7 @@
         <v>1028</v>
       </c>
       <c r="G25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
@@ -1757,16 +1840,19 @@
         <v>87</v>
       </c>
       <c r="J25" t="s">
+        <v>167</v>
+      </c>
+      <c r="K25" t="s">
         <v>168</v>
-      </c>
-      <c r="K25" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>158</v>
       </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -1790,10 +1876,10 @@
         <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K26" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add data organization files for urdu
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DE8932-4E1D-4600-A800-87238592BB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA01D3C1-785D-4C33-868D-92A003E0D6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="178">
   <si>
     <t>Lang.</t>
   </si>
@@ -579,6 +579,12 @@
   </si>
   <si>
     <t>Toronto English; single words</t>
+  </si>
+  <si>
+    <t>Urdu</t>
+  </si>
+  <si>
+    <t>expected 38 unique speakers, but only found 29; but the expected number of utterances was found</t>
   </si>
 </sst>
 </file>
@@ -942,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1886,9 +1892,36 @@
       <c r="A27" t="s">
         <v>159</v>
       </c>
-      <c r="H27" t="str">
+      <c r="B27" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <v>200</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+      <c r="G27" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="0"/>
-        <v/>
+        <v>400</v>
+      </c>
+      <c r="I27">
+        <v>29</v>
+      </c>
+      <c r="J27" t="s">
+        <v>145</v>
+      </c>
+      <c r="K27" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add data organization files for MESS
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B89EB2-65FB-42AA-B193-71998BFCBCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06C1362-8F50-49CB-8FF4-DE84E2D3BEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1727,12 +1727,24 @@
       <c r="C22" t="s">
         <v>4</v>
       </c>
+      <c r="D22">
+        <v>900</v>
+      </c>
+      <c r="E22">
+        <v>900</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
       <c r="G22" t="s">
         <v>35</v>
       </c>
-      <c r="H22" t="str">
+      <c r="H22">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1800</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
Add two more datasets, partially update readme, and upload some vivae docs
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06C1362-8F50-49CB-8FF4-DE84E2D3BEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5142C62D-3A35-407C-9C4E-D9D21F252170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="183">
   <si>
     <t>Lang.</t>
   </si>
@@ -594,6 +594,12 @@
   </si>
   <si>
     <t>angry, sad, calm, happy</t>
+  </si>
+  <si>
+    <t>MAV</t>
+  </si>
+  <si>
+    <t>LimaCastroScott</t>
   </si>
 </sst>
 </file>
@@ -956,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,7 +1039,7 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H29" si="0">IF(OR(ISBLANK(D2), ISBLANK(E2),ISBLANK(F2)), "", SUM(D2:F2))</f>
+        <f t="shared" ref="H2:H31" si="0">IF(OR(ISBLANK(D2), ISBLANK(E2),ISBLANK(F2)), "", SUM(D2:F2))</f>
         <v>605</v>
       </c>
       <c r="I2">
@@ -1647,334 +1653,355 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>124</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>170</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>797</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>0</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>35</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <v>134</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K21" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>125</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>170</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>3086</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <v>4186</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>6430</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>35</v>
       </c>
-      <c r="H21">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>13702</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>356</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>178</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>171</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>900</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>900</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>0</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G24" t="s">
         <v>35</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>6</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>154</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>171</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>62</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>302</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>70</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G25" t="s">
         <v>37</v>
       </c>
-      <c r="H23">
+      <c r="H25">
         <f t="shared" si="0"/>
         <v>434</v>
       </c>
-      <c r="I23">
+      <c r="I25">
         <v>32</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K25" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>155</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>171</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>376</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <v>1512</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <v>564</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>35</v>
       </c>
-      <c r="H24">
+      <c r="H26">
         <f t="shared" si="0"/>
         <v>2452</v>
       </c>
-      <c r="I24">
+      <c r="I26">
         <v>24</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K26" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>156</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>171</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D25">
-        <v>61</v>
-      </c>
-      <c r="E25">
+      <c r="D27">
+        <v>61</v>
+      </c>
+      <c r="E27">
         <v>306</v>
       </c>
-      <c r="F25">
+      <c r="F27">
         <v>121</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>35</v>
       </c>
-      <c r="H25">
+      <c r="H27">
         <f t="shared" si="0"/>
         <v>488</v>
       </c>
-      <c r="I25">
+      <c r="I27">
         <f>4+7</f>
         <v>11</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J27" t="s">
         <v>165</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K27" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>157</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>170</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>4</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <v>201</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <v>1771</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>1028</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G28" t="s">
         <v>166</v>
       </c>
-      <c r="H26">
+      <c r="H28">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>87</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J28" t="s">
         <v>167</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K28" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>158</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>171</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="D27">
+      <c r="D29">
         <v>800</v>
       </c>
-      <c r="E27">
+      <c r="E29">
         <v>1600</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <v>400</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>35</v>
       </c>
-      <c r="H27">
+      <c r="H29">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="I27">
+      <c r="I29">
         <v>2</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J29" t="s">
         <v>169</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K29" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>159</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>170</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>11</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>100</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>200</v>
       </c>
-      <c r="F28">
+      <c r="F30">
         <v>100</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>176</v>
       </c>
-      <c r="H28">
+      <c r="H30">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="I28">
+      <c r="I30">
         <v>29</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J30" t="s">
         <v>145</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K30" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>160</v>
       </c>
-      <c r="H29" t="str">
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Add vivae organization files
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E50953A-E4B5-4526-A29B-B60B95553903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD51DD-A692-4221-8CAB-5EF26EE1ACD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="194">
   <si>
     <t>Lang.</t>
   </si>
@@ -68,9 +68,6 @@
     <t># neg.</t>
   </si>
   <si>
-    <t>anad</t>
-  </si>
-  <si>
     <t>Arabic</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
   </si>
   <si>
     <t>fea</t>
-  </si>
-  <si>
-    <t>from online talk shows; used unsegmented (utterance level); labels no good</t>
   </si>
   <si>
     <t>Sadnes</t>
@@ -611,7 +605,34 @@
     <t>English*</t>
   </si>
   <si>
-    <t>only 1 Canadian speaker; calm is positive here; recoded 91 calm samples as neutral</t>
+    <t>0 or 1</t>
+  </si>
+  <si>
+    <t>calm is positive here; recoded 91 calm samples as neutral</t>
+  </si>
+  <si>
+    <t>achievement</t>
+  </si>
+  <si>
+    <t>ach</t>
+  </si>
+  <si>
+    <t>pleasure</t>
+  </si>
+  <si>
+    <t>ple</t>
+  </si>
+  <si>
+    <t>pain</t>
+  </si>
+  <si>
+    <t>pai</t>
+  </si>
+  <si>
+    <t>non-speech vocalizations; surprise is positive here</t>
+  </si>
+  <si>
+    <t>anger, fear, pain, achievement, pleasure, surprise</t>
   </si>
 </sst>
 </file>
@@ -974,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,10 +1016,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1010,7 +1031,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1019,10 +1040,10 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1033,7 +1054,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1051,74 +1072,89 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H31" si="0">IF(OR(ISBLANK(D2), ISBLANK(E2),ISBLANK(F2)), "", SUM(D2:F2))</f>
+        <f t="shared" ref="H2:H30" si="0">IF(OR(ISBLANK(D2), ISBLANK(E2),ISBLANK(F2)), "", SUM(D2:F2))</f>
         <v>605</v>
       </c>
       <c r="I2">
         <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>228</v>
+      </c>
+      <c r="E3">
+        <v>891</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="str">
+        <v>24</v>
+      </c>
+      <c r="H3">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1304</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>129</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>228</v>
+        <v>36</v>
       </c>
       <c r="E4">
-        <v>891</v>
+        <v>86</v>
       </c>
       <c r="F4">
-        <v>185</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1304</v>
+        <v>128</v>
       </c>
       <c r="I4">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="J4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1126,253 +1162,253 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E5">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="I5">
-        <v>147</v>
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>125</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>720</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <f>6*12</f>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="I6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" t="s">
-        <v>132</v>
+        <v>936</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="K6" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>144</v>
+        <v>1245</v>
       </c>
       <c r="E7">
-        <v>720</v>
+        <v>4541</v>
       </c>
       <c r="F7">
-        <f>6*12</f>
-        <v>72</v>
+        <v>1087</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>936</v>
+        <v>6873</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>1245</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>4541</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>1087</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>6873</v>
+        <v>6</v>
       </c>
       <c r="I8">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K8" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>232</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>493</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>867</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="E10">
-        <v>493</v>
+        <f>535-(79+71)</f>
+        <v>385</v>
       </c>
       <c r="F10">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>867</v>
+        <v>535</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K10" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>71</v>
+        <v>523</v>
       </c>
       <c r="E11">
-        <f>535-(79+71)</f>
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="F11">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>535</v>
+        <v>937</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K11" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1380,35 +1416,35 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>523</v>
+        <v>147</v>
       </c>
       <c r="E12">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="F12">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>937</v>
+        <v>622</v>
       </c>
       <c r="I12">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K12" t="s">
-        <v>151</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1416,101 +1452,101 @@
         <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13">
-        <v>147</v>
+        <v>1317</v>
       </c>
       <c r="E13">
-        <v>333</v>
+        <v>2287</v>
       </c>
       <c r="F13">
-        <v>142</v>
+        <v>1568</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>622</v>
+        <v>5172</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>1317</v>
+        <v>213</v>
       </c>
       <c r="E14">
-        <v>2287</v>
+        <v>1080</v>
       </c>
       <c r="F14">
-        <v>1568</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>5172</v>
+        <v>1293</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K14" t="s">
         <v>140</v>
-      </c>
-      <c r="K14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>213</v>
+        <v>3500</v>
       </c>
       <c r="E15">
-        <v>1080</v>
+        <v>10500</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>1293</v>
+        <v>17500</v>
       </c>
       <c r="I15">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>141</v>
@@ -1521,10 +1557,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1539,7 +1575,7 @@
         <v>3500</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
@@ -1549,10 +1585,10 @@
         <v>10</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1560,35 +1596,35 @@
         <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17">
-        <v>3500</v>
+        <v>132</v>
       </c>
       <c r="E17">
-        <v>10500</v>
+        <v>297</v>
       </c>
       <c r="F17">
-        <v>3500</v>
+        <v>150</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>17500</v>
+        <v>579</v>
       </c>
       <c r="I17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>143</v>
       </c>
       <c r="K17" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1596,393 +1632,393 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18">
-        <v>132</v>
+        <v>480</v>
       </c>
       <c r="E18">
-        <v>297</v>
+        <v>960</v>
       </c>
       <c r="F18">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>579</v>
+        <v>1680</v>
       </c>
       <c r="I18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K18" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19">
-        <v>480</v>
-      </c>
-      <c r="E19">
-        <v>960</v>
-      </c>
-      <c r="F19">
-        <v>240</v>
-      </c>
       <c r="G19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>1680</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="J19" s="1"/>
       <c r="K19" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>797</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>183</v>
-      </c>
-      <c r="J20" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>797</v>
+      </c>
+      <c r="I20">
+        <v>134</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="K20" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>797</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>797</v>
-      </c>
-      <c r="I21">
-        <v>134</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="J21" s="1"/>
       <c r="K21" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
+      <c r="D22">
+        <v>3086</v>
+      </c>
+      <c r="E22">
+        <v>4186</v>
+      </c>
+      <c r="F22">
+        <v>6430</v>
+      </c>
       <c r="G22" t="s">
-        <v>184</v>
-      </c>
-      <c r="J22" s="1"/>
-      <c r="K22" t="s">
-        <v>182</v>
+        <v>34</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>13702</v>
+      </c>
+      <c r="I22">
+        <v>356</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23">
-        <v>3086</v>
+        <v>809</v>
       </c>
       <c r="E23">
-        <v>4186</v>
+        <v>900</v>
       </c>
       <c r="F23">
-        <v>6430</v>
+        <v>91</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>13702</v>
+        <v>1800</v>
       </c>
       <c r="I23">
-        <v>356</v>
+        <v>6</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>152</v>
+        <v>177</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24">
-        <v>809</v>
+        <v>62</v>
       </c>
       <c r="E24">
-        <v>900</v>
+        <v>302</v>
       </c>
       <c r="F24">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>434</v>
       </c>
       <c r="I24">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>186</v>
+        <v>151</v>
+      </c>
+      <c r="K24" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25">
-        <v>62</v>
+        <v>376</v>
       </c>
       <c r="E25">
-        <v>302</v>
+        <v>1512</v>
       </c>
       <c r="F25">
-        <v>70</v>
+        <v>564</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
-        <v>434</v>
+        <v>2452</v>
       </c>
       <c r="I25">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="K25" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26">
-        <v>376</v>
+        <v>61</v>
       </c>
       <c r="E26">
-        <v>1512</v>
+        <v>306</v>
       </c>
       <c r="F26">
-        <v>564</v>
+        <v>121</v>
       </c>
       <c r="G26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>2452</v>
+        <v>488</v>
       </c>
       <c r="I26">
-        <v>24</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>161</v>
+        <f>4+7</f>
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>163</v>
       </c>
       <c r="K26" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27">
-        <v>61</v>
+        <v>201</v>
       </c>
       <c r="E27">
-        <v>306</v>
+        <v>1771</v>
       </c>
       <c r="F27">
-        <v>121</v>
+        <v>1028</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>488</v>
+        <v>3000</v>
       </c>
       <c r="I27">
-        <f>4+7</f>
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="J27" t="s">
         <v>165</v>
       </c>
       <c r="K27" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28">
-        <v>201</v>
+        <v>800</v>
       </c>
       <c r="E28">
-        <v>1771</v>
+        <v>1600</v>
       </c>
       <c r="F28">
-        <v>1028</v>
+        <v>400</v>
       </c>
       <c r="G28" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>2800</v>
       </c>
       <c r="I28">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="J28" t="s">
         <v>167</v>
       </c>
       <c r="K28" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D29">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="E29">
-        <v>1600</v>
+        <v>200</v>
       </c>
       <c r="F29">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>2800</v>
+        <v>400</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J29" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="K29" t="s">
         <v>175</v>
@@ -1990,59 +2026,38 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="E30">
-        <v>200</v>
+        <v>535</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>1085</v>
       </c>
       <c r="I30">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J30" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="K30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" t="s">
-        <v>185</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="K31" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2053,7 +2068,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4FBC7C-E990-492C-91F7-722D544A6419}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2061,58 +2076,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2122,11 +2151,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2136,134 +2163,156 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2276,9 +2325,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2287,299 +2338,310 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2592,10 +2654,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2606,46 +2668,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2670,58 +2721,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data organization files for LimaCastroScott
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FD51DD-A692-4221-8CAB-5EF26EE1ACD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55C6A60-774B-41AF-8C41-7DD03070B3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="199">
   <si>
     <t>Lang.</t>
   </si>
@@ -633,6 +633,21 @@
   </si>
   <si>
     <t>anger, fear, pain, achievement, pleasure, surprise</t>
+  </si>
+  <si>
+    <t>amusement</t>
+  </si>
+  <si>
+    <t>relief</t>
+  </si>
+  <si>
+    <t>rel</t>
+  </si>
+  <si>
+    <t>anger, disgust, fear, sadness, achievement, amusement, pleasure, relief</t>
+  </si>
+  <si>
+    <t>4 pos 4 neg; discarded four for valence mismatch: relief_MS_13, relief_MS_14, relief_MS_15, fear_T_16</t>
   </si>
 </sst>
 </file>
@@ -997,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1673,12 +1688,30 @@
       <c r="C19" t="s">
         <v>4</v>
       </c>
+      <c r="D19">
+        <v>59</v>
+      </c>
+      <c r="E19">
+        <v>58</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
       <c r="G19" t="s">
         <v>181</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="K19" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2151,9 +2184,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2313,6 +2348,28 @@
       </c>
       <c r="C14" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2327,9 +2384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Add data organization files for MAV and update readme
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55C6A60-774B-41AF-8C41-7DD03070B3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6183BD33-5C2D-4DEB-A9B2-BD8DF9C1A7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="202">
   <si>
     <t>Lang.</t>
   </si>
@@ -648,6 +648,15 @@
   </si>
   <si>
     <t>4 pos 4 neg; discarded four for valence mismatch: relief_MS_13, relief_MS_14, relief_MS_15, fear_T_16</t>
+  </si>
+  <si>
+    <t>pleased</t>
+  </si>
+  <si>
+    <t>painful</t>
+  </si>
+  <si>
+    <t>anger, disgust, fear, pain, sadness, surprise, happiness, pleasure, neutral</t>
   </si>
 </sst>
 </file>
@@ -1010,11 +1019,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1023,7 +1030,7 @@
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" customWidth="1"/>
@@ -1760,10 +1767,28 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
       <c r="G21" t="s">
         <v>182</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="K21" t="s">
         <v>180</v>
       </c>
@@ -2091,6 +2116,28 @@
       </c>
       <c r="K30" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <f t="shared" ref="D31:F31" si="1">SUM(D2:D30)</f>
+        <v>18062</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>46177</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>19538</v>
+      </c>
+      <c r="H31">
+        <f>SUM(H2:H30)</f>
+        <v>83777</v>
+      </c>
+      <c r="I31">
+        <f>SUM(I2:I30)</f>
+        <v>1148</v>
       </c>
     </row>
   </sheetData>
@@ -2184,11 +2231,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2372,6 +2417,17 @@
         <v>196</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B5">
     <sortCondition ref="A2:A5"/>
@@ -2382,7 +2438,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2696,6 +2752,17 @@
         <v>60</v>
       </c>
       <c r="C28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2711,9 +2778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Fix LEGOv2 organization files, document sample rates, remove a gitignore, and update notes
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6183BD33-5C2D-4DEB-A9B2-BD8DF9C1A7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA477E8-5B72-4BDD-BE36-75BBFFFCD8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_retained" sheetId="1" r:id="rId1"/>
-    <sheet name="multi-valenced" sheetId="6" r:id="rId2"/>
-    <sheet name="positive" sheetId="2" r:id="rId3"/>
-    <sheet name="negative" sheetId="3" r:id="rId4"/>
-    <sheet name="neutral" sheetId="5" r:id="rId5"/>
-    <sheet name="discard" sheetId="4" r:id="rId6"/>
+    <sheet name="examining_sample_rates" sheetId="9" r:id="rId2"/>
+    <sheet name="multi-valenced" sheetId="6" r:id="rId3"/>
+    <sheet name="positive" sheetId="2" r:id="rId4"/>
+    <sheet name="negative" sheetId="3" r:id="rId5"/>
+    <sheet name="neutral" sheetId="5" r:id="rId6"/>
+    <sheet name="discard" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId8"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="208">
   <si>
     <t>Lang.</t>
   </si>
@@ -299,9 +303,6 @@
     <t>boredom is negative; data from kaggle link, not the one provided in the paper</t>
   </si>
   <si>
-    <t>perceived valence recoded to majority and average votes; if either matched intended valence, sample kept; discarded 58</t>
-  </si>
-  <si>
     <t>bor</t>
   </si>
   <si>
@@ -474,12 +475,6 @@
   </si>
   <si>
     <t>angry, anxious, neutral, sad, worried, apologetic, pensive, excited, enthusiastic,  happy</t>
-  </si>
-  <si>
-    <t>very angry, slightly angry, non-angry</t>
-  </si>
-  <si>
-    <t>only angry</t>
   </si>
   <si>
     <t>New Zealand English; valence labels were provided for the non-primary emotions; semi-natural elicitation (almost spont.); apologetic, anxious, worried negative; excited and happy positive; not all present</t>
@@ -658,12 +653,42 @@
   <si>
     <t>anger, disgust, fear, pain, sadness, surprise, happiness, pleasure, neutral</t>
   </si>
+  <si>
+    <t>sample_rate (kHz)</t>
+  </si>
+  <si>
+    <t>perceived valence recoded to majority and average votes; if either matched intended valence, sample kept; discarded 58; 12-bit depth</t>
+  </si>
+  <si>
+    <t>friendly</t>
+  </si>
+  <si>
+    <t>fri</t>
+  </si>
+  <si>
+    <t>only angry, friendly, neutral, kept</t>
+  </si>
+  <si>
+    <t>very angry, slightly angry, neutral, friendly, garbage</t>
+  </si>
+  <si>
+    <t>Sum of n</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +698,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -697,17 +729,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -720,6 +760,1439 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dataset_details.xlsx]examining_sample_rates!PivotTable2</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>examining_sample_rates!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>examining_sample_rates!$A$4:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>examining_sample_rates!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10282</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18954</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-31BD-49DE-AF9B-240510535293}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCAD6D8-3279-4D8C-8680-04C278F7374C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="m c" refreshedDate="44462.757387152778" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="29" xr:uid="{3F90611D-DE44-42DF-861A-38E3617B3766}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:I30" sheet="samples_retained"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="sample_rate (kHz)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="8" maxValue="192" count="7">
+        <n v="44.1"/>
+        <n v="48"/>
+        <n v="192"/>
+        <n v="16"/>
+        <n v="22.05"/>
+        <n v="8"/>
+        <n v="24.4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="elicited from discourse" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Elicit." numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="# pos." numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="3500"/>
+    </cacheField>
+    <cacheField name="# neg." numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="10500"/>
+    </cacheField>
+    <cacheField name="# neu." numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="6430"/>
+    </cacheField>
+    <cacheField name="Lang." numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="n" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="6" maxValue="17500"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="119"/>
+    <n v="486"/>
+    <n v="0"/>
+    <s v="Greek"/>
+    <n v="605"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="non-discourse"/>
+    <s v="acted + spon."/>
+    <n v="228"/>
+    <n v="891"/>
+    <n v="185"/>
+    <s v="Turkish"/>
+    <n v="1304"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="discourse"/>
+    <s v="acted"/>
+    <n v="36"/>
+    <n v="86"/>
+    <n v="6"/>
+    <s v="Turkish"/>
+    <n v="128"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="discourse"/>
+    <s v="acted"/>
+    <n v="49"/>
+    <n v="13"/>
+    <n v="13"/>
+    <s v="English"/>
+    <n v="75"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="144"/>
+    <n v="720"/>
+    <n v="72"/>
+    <s v="French"/>
+    <n v="936"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="1245"/>
+    <n v="4541"/>
+    <n v="1087"/>
+    <s v="English"/>
+    <n v="6873"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <s v="English"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="spon."/>
+    <n v="232"/>
+    <n v="493"/>
+    <n v="142"/>
+    <s v="Estonian"/>
+    <n v="867"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="71"/>
+    <n v="385"/>
+    <n v="79"/>
+    <s v="German"/>
+    <n v="535"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="discourse"/>
+    <s v="spon."/>
+    <n v="523"/>
+    <n v="376"/>
+    <n v="38"/>
+    <s v="English"/>
+    <n v="937"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="147"/>
+    <n v="333"/>
+    <n v="142"/>
+    <s v="English"/>
+    <n v="622"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="1317"/>
+    <n v="2287"/>
+    <n v="1568"/>
+    <s v="English"/>
+    <n v="5172"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="non-discourse"/>
+    <s v="spon."/>
+    <n v="213"/>
+    <n v="1080"/>
+    <n v="0"/>
+    <s v="English"/>
+    <n v="1293"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="3500"/>
+    <n v="10500"/>
+    <n v="3500"/>
+    <s v="English"/>
+    <n v="17500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="3500"/>
+    <n v="10500"/>
+    <n v="3500"/>
+    <s v="Mandarin Chinese"/>
+    <n v="17500"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="discourse"/>
+    <s v="acted"/>
+    <n v="132"/>
+    <n v="297"/>
+    <n v="150"/>
+    <s v="Arabic"/>
+    <n v="579"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="480"/>
+    <n v="960"/>
+    <n v="240"/>
+    <s v="English"/>
+    <n v="1680"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="59"/>
+    <n v="58"/>
+    <n v="0"/>
+    <s v="Portuguese*"/>
+    <n v="117"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="discourse"/>
+    <s v="spon."/>
+    <n v="4"/>
+    <n v="934"/>
+    <n v="3305"/>
+    <s v="English"/>
+    <n v="4243"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="20"/>
+    <n v="60"/>
+    <n v="10"/>
+    <s v="French*"/>
+    <n v="90"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="discourse"/>
+    <s v="acted"/>
+    <n v="3086"/>
+    <n v="4186"/>
+    <n v="6430"/>
+    <s v="English"/>
+    <n v="13702"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="809"/>
+    <n v="900"/>
+    <n v="91"/>
+    <s v="English"/>
+    <n v="1800"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="62"/>
+    <n v="302"/>
+    <n v="70"/>
+    <s v="French"/>
+    <n v="434"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="376"/>
+    <n v="1512"/>
+    <n v="564"/>
+    <s v="English"/>
+    <n v="2452"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="61"/>
+    <n v="306"/>
+    <n v="121"/>
+    <s v="English"/>
+    <n v="488"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="discourse"/>
+    <s v="acted"/>
+    <n v="201"/>
+    <n v="1771"/>
+    <n v="1028"/>
+    <s v="Persian"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="800"/>
+    <n v="1600"/>
+    <n v="400"/>
+    <s v="English"/>
+    <n v="2800"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="discourse"/>
+    <s v="spon."/>
+    <n v="100"/>
+    <n v="200"/>
+    <n v="100"/>
+    <s v="Urdu"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="non-discourse"/>
+    <s v="acted"/>
+    <n v="550"/>
+    <n v="535"/>
+    <n v="0"/>
+    <s v="English*"/>
+    <n v="1085"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24F4754D-EF09-426F-B469-71FEBBD3E589}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="5"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of n" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1019,287 +2492,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+    <col min="2" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="6" width="5.88671875" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
-        <v>124</v>
-      </c>
       <c r="J1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>169</v>
+      <c r="B2">
+        <v>44.1</v>
       </c>
       <c r="C2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>119</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>486</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H30" si="0">IF(OR(ISBLANK(D2), ISBLANK(E2),ISBLANK(F2)), "", SUM(D2:F2))</f>
+      <c r="I2">
+        <f t="shared" ref="I2:I30" si="0">IF(OR(ISBLANK(E2), ISBLANK(F2),ISBLANK(G2)), "", SUM(E2:G2))</f>
         <v>605</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
-        <v>148</v>
-      </c>
       <c r="K2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>169</v>
+      <c r="B3">
+        <v>48</v>
       </c>
       <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>228</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>891</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>185</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <f t="shared" si="0"/>
         <v>1304</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
-        <v>129</v>
-      </c>
       <c r="K3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>168</v>
+      <c r="B4">
+        <v>48</v>
       </c>
       <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>36</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>86</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>147</v>
       </c>
-      <c r="J4" t="s">
-        <v>130</v>
-      </c>
       <c r="K4" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
-        <v>168</v>
+      <c r="B5">
+        <v>48</v>
       </c>
       <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>49</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
       </c>
       <c r="F5">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="I5" t="s">
-        <v>125</v>
-      </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K5" t="s">
+        <v>129</v>
+      </c>
+      <c r="L5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>169</v>
+      <c r="B6">
+        <v>192</v>
       </c>
       <c r="C6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>144</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>720</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f>6*12</f>
         <v>72</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>36</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>936</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
-        <v>169</v>
+      <c r="B7">
+        <v>16</v>
       </c>
       <c r="C7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1245</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>4541</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1087</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>6873</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>91</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
-        <v>169</v>
+      <c r="B8">
+        <v>22.05</v>
       </c>
       <c r="C8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1307,836 +2801,905 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="s">
-        <v>169</v>
+      <c r="B9">
+        <v>44.1</v>
       </c>
       <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>232</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>493</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>142</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>867</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" t="s">
-        <v>169</v>
+      <c r="B10">
+        <v>16</v>
       </c>
       <c r="C10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>71</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f>535-(79+71)</f>
         <v>385</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>79</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>57</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>10</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
-        <v>168</v>
+      <c r="B11">
+        <v>44.1</v>
       </c>
       <c r="C11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>523</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>376</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>38</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>34</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>937</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>63</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
-        <v>169</v>
+      <c r="B12">
+        <v>16</v>
       </c>
       <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>147</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>333</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>142</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>34</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>622</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>3</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
-      <c r="B13" t="s">
-        <v>169</v>
+      <c r="B13">
+        <v>16</v>
       </c>
       <c r="C13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1317</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>2287</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1568</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>34</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>5172</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>4</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" t="s">
-        <v>169</v>
+      <c r="B14">
+        <v>48</v>
       </c>
       <c r="C14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>213</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1080</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>34</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="0"/>
         <v>1293</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>44</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L14" t="s">
         <v>139</v>
       </c>
-      <c r="K14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" t="s">
-        <v>169</v>
+        <v>101</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
       </c>
       <c r="C15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>3500</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>10500</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>3500</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>34</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="0"/>
         <v>17500</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>10</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L15" t="s">
         <v>141</v>
       </c>
-      <c r="K15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>3500</v>
+      </c>
+      <c r="F16">
+        <v>10500</v>
+      </c>
+      <c r="G16">
+        <v>3500</v>
+      </c>
+      <c r="H16" t="s">
         <v>103</v>
       </c>
-      <c r="B16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>3500</v>
-      </c>
-      <c r="E16">
-        <v>10500</v>
-      </c>
-      <c r="F16">
-        <v>3500</v>
-      </c>
-      <c r="G16" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>17500</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>10</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L16" t="s">
         <v>141</v>
       </c>
-      <c r="K16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" t="s">
-        <v>168</v>
+        <v>104</v>
+      </c>
+      <c r="B17">
+        <v>44.1</v>
       </c>
       <c r="C17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" t="s">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>132</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>297</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>150</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>9</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="0"/>
         <v>579</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>6</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="K17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" t="s">
-        <v>169</v>
+      <c r="B18">
+        <v>44.1</v>
       </c>
       <c r="C18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>480</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>960</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>240</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>34</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>1680</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>4</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L18" t="s">
         <v>144</v>
       </c>
-      <c r="K18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" t="s">
-        <v>169</v>
+        <v>176</v>
+      </c>
+      <c r="B19">
+        <v>44.1</v>
       </c>
       <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>59</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>58</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>0</v>
       </c>
-      <c r="G19" t="s">
-        <v>181</v>
-      </c>
-      <c r="H19">
+      <c r="H19" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>4</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="K19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" t="s">
-        <v>168</v>
+        <v>121</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
       </c>
       <c r="C20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
       <c r="E20">
-        <v>797</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
+        <v>934</v>
+      </c>
+      <c r="G20">
+        <v>3305</v>
+      </c>
+      <c r="H20" t="s">
         <v>34</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="0"/>
-        <v>797</v>
-      </c>
-      <c r="I20">
+        <v>4243</v>
+      </c>
+      <c r="J20">
         <v>134</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" t="s">
-        <v>169</v>
+        <v>175</v>
+      </c>
+      <c r="B21">
+        <v>44.1</v>
       </c>
       <c r="C21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>20</v>
       </c>
-      <c r="E21">
-        <v>60</v>
-      </c>
       <c r="F21">
+        <v>60</v>
+      </c>
+      <c r="G21">
         <v>10</v>
       </c>
-      <c r="G21" t="s">
-        <v>182</v>
-      </c>
-      <c r="H21">
+      <c r="H21" t="s">
+        <v>179</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>10</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K21" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" t="s">
-        <v>168</v>
+        <v>122</v>
+      </c>
+      <c r="B22">
+        <v>48</v>
       </c>
       <c r="C22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>3086</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>4186</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>6430</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>34</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>13702</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>356</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="B23">
+        <v>24.4</v>
       </c>
       <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>809</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>900</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>91</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>34</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>6</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>152</v>
-      </c>
-      <c r="B24" t="s">
-        <v>169</v>
+        <v>149</v>
+      </c>
+      <c r="B24">
+        <v>44.1</v>
       </c>
       <c r="C24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>62</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>302</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>70</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>36</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f t="shared" si="0"/>
         <v>434</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>32</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="K24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B25" t="s">
-        <v>169</v>
+        <v>150</v>
+      </c>
+      <c r="B25">
+        <v>48</v>
       </c>
       <c r="C25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" t="s">
         <v>4</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>376</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>1512</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>564</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>34</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>2452</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>24</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>154</v>
-      </c>
-      <c r="B26" t="s">
-        <v>169</v>
+        <v>151</v>
+      </c>
+      <c r="B26">
+        <v>44.1</v>
       </c>
       <c r="C26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>61</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>306</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>121</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>34</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f t="shared" si="0"/>
         <v>488</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f>4+7</f>
         <v>11</v>
       </c>
-      <c r="J26" t="s">
-        <v>163</v>
-      </c>
       <c r="K26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="L26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" t="s">
-        <v>168</v>
+        <v>152</v>
+      </c>
+      <c r="B27">
+        <v>44.1</v>
       </c>
       <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" t="s">
         <v>4</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>201</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>1771</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>1028</v>
       </c>
-      <c r="G27" t="s">
-        <v>164</v>
-      </c>
-      <c r="H27">
+      <c r="H27" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>87</v>
       </c>
-      <c r="J27" t="s">
-        <v>165</v>
-      </c>
       <c r="K27" t="s">
+        <v>162</v>
+      </c>
+      <c r="L27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28">
+        <v>24.4</v>
+      </c>
+      <c r="C28" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>800</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>1600</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>400</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>34</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>2</v>
       </c>
-      <c r="J28" t="s">
-        <v>167</v>
-      </c>
       <c r="K28" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="L28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" t="s">
-        <v>168</v>
+        <v>154</v>
+      </c>
+      <c r="B29">
+        <v>44.1</v>
       </c>
       <c r="C29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" t="s">
         <v>10</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>100</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>200</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>100</v>
       </c>
-      <c r="G29" t="s">
-        <v>174</v>
-      </c>
-      <c r="H29">
+      <c r="H29" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>29</v>
       </c>
-      <c r="J29" t="s">
-        <v>143</v>
-      </c>
       <c r="K29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="L29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" t="s">
-        <v>169</v>
+        <v>155</v>
+      </c>
+      <c r="B30">
+        <v>44.1</v>
       </c>
       <c r="C30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" t="s">
         <v>4</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>550</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>535</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>0</v>
       </c>
-      <c r="G30" t="s">
-        <v>183</v>
-      </c>
-      <c r="H30">
+      <c r="H30" t="s">
+        <v>180</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="0"/>
         <v>1085</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>11</v>
       </c>
-      <c r="J30" t="s">
-        <v>193</v>
-      </c>
       <c r="K30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D31">
-        <f t="shared" ref="D31:F31" si="1">SUM(D2:D30)</f>
-        <v>18062</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="L30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E31">
-        <f t="shared" si="1"/>
-        <v>46177</v>
+        <f t="shared" ref="E31:G31" si="1">SUM(E2:E30)</f>
+        <v>18066</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>19538</v>
-      </c>
-      <c r="H31">
-        <f>SUM(H2:H30)</f>
-        <v>83777</v>
+        <v>46314</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>22843</v>
       </c>
       <c r="I31">
         <f>SUM(I2:I30)</f>
+        <v>87223</v>
+      </c>
+      <c r="J31">
+        <f>SUM(J2:J30)</f>
         <v>1148</v>
       </c>
     </row>
@@ -2147,6 +3710,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBFB79-63BD-404D-BA2E-15C291EEF33C}">
+  <dimension ref="A3:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4243</v>
+      </c>
+      <c r="C4" s="7">
+        <f>B4/$B$11</f>
+        <v>4.8645426091741856E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4">
+        <v>48202</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" ref="C5:C10" si="0">B5/$B$11</f>
+        <v>0.55262946699838345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>22.05</v>
+      </c>
+      <c r="B6" s="4">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>6.8789195510358508E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>24.4</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4600</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>5.2738383224608186E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>44.1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>10282</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.11788175137291769</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18954</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.21730506861722251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>192</v>
+      </c>
+      <c r="B10" s="4">
+        <v>936</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0731114499615927E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="4">
+        <v>87223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4FBC7C-E990-492C-91F7-722D544A6419}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2156,16 +3838,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>96</v>
-      </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2176,10 +3858,10 @@
         <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2190,10 +3872,10 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2204,24 +3886,24 @@
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2229,9 +3911,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE94AD6F-649F-4002-92D4-6F52AF8E9D45}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2304,7 +3986,7 @@
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2315,18 +3997,18 @@
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
         <v>93</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2337,95 +4019,106 @@
         <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
         <v>108</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>110</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B14" t="s">
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
         <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
         <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2436,7 +4129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA86EBB-7E83-4F5A-91CB-F1C7A25C89A4}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2653,7 +4346,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -2664,7 +4357,7 @@
         <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2675,29 +4368,29 @@
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
         <v>91</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -2708,62 +4401,62 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
         <v>112</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
         <v>114</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
         <v>116</v>
-      </c>
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s">
         <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2774,7 +4467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E52F00-6B74-4EB8-92AB-C7069E726720}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2827,7 +4520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CA4603-F405-47FD-B096-17B0BE7B1580}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2873,7 +4566,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
@@ -2881,7 +4574,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -2889,7 +4582,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Account for two corrupt files
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification_datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA477E8-5B72-4BDD-BE36-75BBFFFCD8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE334AB-BC1B-4AEC-A85D-BFA4C84A8F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -686,7 +686,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -743,7 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,6 +870,202 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -903,6 +1099,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -918,6 +1119,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -933,6 +1139,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -948,6 +1159,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -963,6 +1179,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -978,6 +1199,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -995,6 +1221,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-84E8-4EB5-A081-A5A596A35FFA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2114,7 +2345,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24F4754D-EF09-426F-B469-71FEBBD3E589}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24F4754D-EF09-426F-B469-71FEBBD3E589}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -2172,12 +2403,96 @@
   <dataFields count="1">
     <dataField name="Sum of n" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="8">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -2494,7 +2809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8DFBC8-91B8-4BE5-BB9F-4B527424BFF3}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2564,7 +2881,7 @@
         <v>119</v>
       </c>
       <c r="F2">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2574,7 +2891,7 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I30" si="0">IF(OR(ISBLANK(E2), ISBLANK(F2),ISBLANK(G2)), "", SUM(E2:G2))</f>
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J2">
         <v>6</v>
@@ -3349,14 +3666,14 @@
         <v>4186</v>
       </c>
       <c r="G22">
-        <v>6430</v>
+        <v>6429</v>
       </c>
       <c r="H22" t="s">
         <v>34</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>13702</v>
+        <v>13701</v>
       </c>
       <c r="J22">
         <v>356</v>
@@ -3688,15 +4005,15 @@
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>46314</v>
+        <v>46313</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>22843</v>
+        <v>22842</v>
       </c>
       <c r="I31">
         <f>SUM(I2:I30)</f>
-        <v>87223</v>
+        <v>87221</v>
       </c>
       <c r="J31">
         <f>SUM(J2:J30)</f>
@@ -4335,7 +4652,7 @@
         <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Improve formatting in readme and update speaker counts in notes
</commit_message>
<xml_diff>
--- a/datasets/dataset_details.xlsx
+++ b/datasets/dataset_details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\replace_me\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\code_temp\final_commit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722274B3-CA50-429D-BCE7-CCDAE7C3F48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E848EF-1581-41A1-8FB5-9756E99BB6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E237FE3-C83C-412B-869E-6816986B07DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="3" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3009,7 +3009,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F4611FE3-0A41-4C73-B23B-2D378539504D}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F4611FE3-0A41-4C73-B23B-2D378539504D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -3735,7 +3735,7 @@
         <v>128</v>
       </c>
       <c r="J4">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K4" t="s">
         <v>129</v>
@@ -4010,7 +4010,7 @@
         <v>937</v>
       </c>
       <c r="J11">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>135</v>
@@ -4127,7 +4127,7 @@
         <v>1293</v>
       </c>
       <c r="J14">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>138</v>
@@ -4322,7 +4322,7 @@
         <v>4243</v>
       </c>
       <c r="J19">
-        <v>134</v>
+        <v>291</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>204</v>
@@ -4439,7 +4439,7 @@
         <v>13701</v>
       </c>
       <c r="J22">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>148</v>
@@ -4780,7 +4780,7 @@
       </c>
       <c r="J31">
         <f>SUM(J2:J30)</f>
-        <v>1148</v>
+        <v>1307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>